<commit_message>
alteração da matriz de rastreabilidade
</commit_message>
<xml_diff>
--- a/docs/ARTEFATOS(15-23)/ARTEFATOS(19,22,23)/MATRIZ_DE_RASTREABILIDADE.xlsx
+++ b/docs/ARTEFATOS(15-23)/ARTEFATOS(19,22,23)/MATRIZ_DE_RASTREABILIDADE.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi6NEPEaOPm3ofSuTZsxJoFT0C8eA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjGH0yettrDsx7jf9Sk/QEl7x3w1Q=="/>
     </ext>
   </extLst>
 </workbook>
@@ -472,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -480,7 +480,7 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -492,10 +492,10 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -503,49 +503,46 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,17 +967,17 @@
       <c r="AE3" s="9"/>
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
-      <c r="AH3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AH3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="AJ3" s="9"/>
       <c r="AK3" s="9"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
       <c r="AO3" s="9"/>
       <c r="AP3" s="9"/>
       <c r="AQ3" s="9"/>
@@ -995,10 +992,10 @@
       <c r="AZ3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>2.0</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="8"/>
@@ -1027,27 +1024,27 @@
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="10" t="s">
+      <c r="AC4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AD4" s="9"/>
-      <c r="AE4" s="10" t="s">
+      <c r="AE4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AF4" s="9"/>
       <c r="AG4" s="9"/>
       <c r="AH4" s="9"/>
       <c r="AI4" s="9"/>
-      <c r="AJ4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM4" s="10" t="s">
+      <c r="AJ4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AN4" s="9"/>
@@ -1068,7 +1065,7 @@
       <c r="A5" s="6">
         <v>3.0</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="8"/>
@@ -1103,17 +1100,17 @@
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
       <c r="AH5" s="9"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM5" s="10" t="s">
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM5" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AN5" s="9"/>
@@ -1131,10 +1128,10 @@
       <c r="AZ5" s="9"/>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>4.0</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="8"/>
@@ -1170,16 +1167,16 @@
       <c r="AG6" s="9"/>
       <c r="AH6" s="9"/>
       <c r="AI6" s="9"/>
-      <c r="AJ6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM6" s="10" t="s">
+      <c r="AJ6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM6" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AN6" s="9"/>
@@ -1197,10 +1194,10 @@
       <c r="AZ6" s="9"/>
     </row>
     <row r="7" ht="63.0" customHeight="1">
-      <c r="A7" s="16">
+      <c r="A7" s="8">
         <v>5.0</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>57</v>
       </c>
       <c r="C7" s="8"/>
@@ -1229,37 +1226,37 @@
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
       <c r="AB7" s="9"/>
-      <c r="AC7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF7" s="10" t="s">
+      <c r="AC7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AG7" s="9"/>
       <c r="AH7" s="9"/>
-      <c r="AI7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM7" s="10" t="s">
+      <c r="AI7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AN7" s="9"/>
-      <c r="AO7" s="10" t="s">
+      <c r="AO7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AP7" s="9"/>
@@ -1275,10 +1272,10 @@
       <c r="AZ7" s="9"/>
     </row>
     <row r="8" ht="72.0" customHeight="1">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>6.0</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="8"/>
@@ -1309,7 +1306,7 @@
       <c r="AB8" s="9"/>
       <c r="AC8" s="9"/>
       <c r="AD8" s="9"/>
-      <c r="AE8" s="10" t="s">
+      <c r="AE8" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AF8" s="9"/>
@@ -1335,10 +1332,10 @@
       <c r="AZ8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="16">
+      <c r="A9" s="8">
         <v>7.0</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="8"/>
@@ -1368,7 +1365,7 @@
       <c r="AA9" s="9"/>
       <c r="AB9" s="9"/>
       <c r="AC9" s="9"/>
-      <c r="AD9" s="10" t="s">
+      <c r="AD9" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AE9" s="9"/>
@@ -1381,10 +1378,10 @@
       <c r="AL9" s="9"/>
       <c r="AM9" s="9"/>
       <c r="AN9" s="9"/>
-      <c r="AO9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP9" s="10" t="s">
+      <c r="AO9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP9" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AQ9" s="9"/>
@@ -1399,10 +1396,10 @@
       <c r="AZ9" s="9"/>
     </row>
     <row r="10" ht="70.5" customHeight="1">
-      <c r="A10" s="13">
+      <c r="A10" s="11">
         <v>8.0</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C10" s="8"/>
@@ -1443,7 +1440,7 @@
       <c r="AL10" s="9"/>
       <c r="AM10" s="9"/>
       <c r="AN10" s="9"/>
-      <c r="AO10" s="10" t="s">
+      <c r="AO10" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AP10" s="9"/>
@@ -1459,27 +1456,27 @@
       <c r="AZ10" s="9"/>
     </row>
     <row r="11" ht="85.5" customHeight="1">
-      <c r="A11" s="16">
+      <c r="A11" s="8">
         <v>9.0</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="10" t="s">
+      <c r="J11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>53</v>
       </c>
       <c r="L11" s="9"/>
@@ -1525,10 +1522,10 @@
       <c r="AZ11" s="9"/>
     </row>
     <row r="12" ht="70.5" customHeight="1">
-      <c r="A12" s="13">
+      <c r="A12" s="11">
         <v>10.0</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C12" s="8"/>
@@ -1536,7 +1533,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>53</v>
       </c>
       <c r="I12" s="9"/>
@@ -1585,46 +1582,46 @@
       <c r="AZ12" s="9"/>
     </row>
     <row r="13" ht="57.75" customHeight="1">
-      <c r="A13" s="16">
+      <c r="A13" s="8">
         <v>11.0</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
       <c r="AI13" s="9"/>
       <c r="AJ13" s="9"/>
       <c r="AK13" s="9"/>
@@ -1645,41 +1642,41 @@
       <c r="AZ13" s="9"/>
     </row>
     <row r="14" ht="47.25" customHeight="1">
-      <c r="A14" s="16">
+      <c r="A14" s="8">
         <v>11.0</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
-      <c r="AH14" s="18"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="9"/>
       <c r="AK14" s="9"/>
@@ -1700,10 +1697,10 @@
       <c r="AZ14" s="9"/>
     </row>
     <row r="15" ht="76.5" customHeight="1">
-      <c r="A15" s="13">
-        <v>13.0</v>
-      </c>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="17">
+        <v>12.0</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="8"/>
@@ -1719,7 +1716,7 @@
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="10" t="s">
+      <c r="P15" s="9" t="s">
         <v>53</v>
       </c>
       <c r="Q15" s="9"/>
@@ -1760,10 +1757,10 @@
       <c r="AZ15" s="9"/>
     </row>
     <row r="16" ht="74.25" customHeight="1">
-      <c r="A16" s="16">
-        <v>14.0</v>
-      </c>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="18">
+        <v>13.0</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="8"/>
@@ -1772,22 +1769,22 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="12"/>
+      <c r="K16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" s="10"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
-      <c r="R16" s="10" t="s">
+      <c r="R16" s="9" t="s">
         <v>53</v>
       </c>
       <c r="S16" s="9"/>
-      <c r="T16" s="10" t="s">
+      <c r="T16" s="9" t="s">
         <v>53</v>
       </c>
       <c r="U16" s="9"/>
@@ -1824,10 +1821,10 @@
       <c r="AZ16" s="9"/>
     </row>
     <row r="17" ht="1.5" customHeight="1">
-      <c r="A17" s="16">
+      <c r="A17" s="8">
         <v>15.0</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1877,10 +1874,10 @@
       <c r="AZ17" s="9"/>
     </row>
     <row r="18" ht="75.0" customHeight="1">
-      <c r="A18" s="13">
-        <v>16.0</v>
-      </c>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="17">
+        <v>14.0</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="8"/>
@@ -1901,10 +1898,10 @@
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
-      <c r="U18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="V18" s="10" t="s">
+      <c r="U18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V18" s="9" t="s">
         <v>53</v>
       </c>
       <c r="W18" s="9"/>
@@ -1939,10 +1936,10 @@
       <c r="AZ18" s="9"/>
     </row>
     <row r="19" ht="71.25" customHeight="1">
-      <c r="A19" s="16">
-        <v>17.0</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="18">
+        <v>15.0</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="8"/>
@@ -1961,7 +1958,7 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
-      <c r="S19" s="10" t="s">
+      <c r="S19" s="9" t="s">
         <v>68</v>
       </c>
       <c r="T19" s="9"/>
@@ -1999,10 +1996,10 @@
       <c r="AZ19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="13">
-        <v>18.0</v>
-      </c>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="17">
+        <v>16.0</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C20" s="8"/>
@@ -2023,24 +2020,24 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
-      <c r="U20" s="11" t="s">
+      <c r="U20" s="10" t="s">
         <v>68</v>
       </c>
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
-      <c r="X20" s="10" t="s">
+      <c r="X20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y20" s="10" t="s">
+      <c r="Y20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Z20" s="10" t="s">
+      <c r="Z20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AA20" s="10" t="s">
+      <c r="AA20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AB20" s="10" t="s">
+      <c r="AB20" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AC20" s="9"/>
@@ -2069,10 +2066,10 @@
       <c r="AZ20" s="9"/>
     </row>
     <row r="21" ht="75.75" customHeight="1">
-      <c r="A21" s="16">
-        <v>19.0</v>
-      </c>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="18">
+        <v>17.0</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C21" s="8"/>
@@ -2093,24 +2090,24 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
-      <c r="U21" s="10" t="s">
+      <c r="U21" s="9" t="s">
         <v>68</v>
       </c>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
-      <c r="X21" s="10" t="s">
+      <c r="X21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y21" s="10" t="s">
+      <c r="Y21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Z21" s="10" t="s">
+      <c r="Z21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AA21" s="10" t="s">
+      <c r="AA21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AB21" s="10" t="s">
+      <c r="AB21" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AC21" s="9"/>
@@ -2139,10 +2136,10 @@
       <c r="AZ21" s="9"/>
     </row>
     <row r="22" ht="60.0" customHeight="1">
-      <c r="A22" s="13">
-        <v>20.0</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="17">
+        <v>18.0</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>71</v>
       </c>
       <c r="C22" s="8"/>
@@ -2163,24 +2160,24 @@
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
-      <c r="U22" s="10" t="s">
+      <c r="U22" s="9" t="s">
         <v>68</v>
       </c>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
-      <c r="X22" s="10" t="s">
+      <c r="X22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y22" s="10" t="s">
+      <c r="Y22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Z22" s="10" t="s">
+      <c r="Z22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AA22" s="10" t="s">
+      <c r="AA22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AB22" s="10" t="s">
+      <c r="AB22" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AC22" s="9"/>
@@ -2209,10 +2206,10 @@
       <c r="AZ22" s="9"/>
     </row>
     <row r="23" ht="60.0" customHeight="1">
-      <c r="A23" s="16">
-        <v>21.0</v>
-      </c>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="18">
+        <v>19.0</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="8"/>
@@ -2233,24 +2230,24 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
-      <c r="U23" s="10" t="s">
+      <c r="U23" s="9" t="s">
         <v>68</v>
       </c>
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
-      <c r="X23" s="10" t="s">
+      <c r="X23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y23" s="10" t="s">
+      <c r="Y23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Z23" s="10" t="s">
+      <c r="Z23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AA23" s="10" t="s">
+      <c r="AA23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AB23" s="10" t="s">
+      <c r="AB23" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AC23" s="9"/>
@@ -2279,10 +2276,10 @@
       <c r="AZ23" s="9"/>
     </row>
     <row r="24" ht="80.25" customHeight="1">
-      <c r="A24" s="13">
-        <v>22.0</v>
-      </c>
-      <c r="B24" s="22" t="s">
+      <c r="A24" s="17">
+        <v>20.0</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C24" s="8"/>
@@ -2325,16 +2322,16 @@
       <c r="AN24" s="9"/>
       <c r="AO24" s="9"/>
       <c r="AP24" s="9"/>
-      <c r="AQ24" s="10" t="s">
+      <c r="AQ24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AR24" s="10" t="s">
+      <c r="AR24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AS24" s="10" t="s">
+      <c r="AS24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AT24" s="10" t="s">
+      <c r="AT24" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AU24" s="9"/>
@@ -2345,10 +2342,10 @@
       <c r="AZ24" s="9"/>
     </row>
     <row r="25" ht="67.5" customHeight="1">
-      <c r="A25" s="6">
-        <v>23.0</v>
-      </c>
-      <c r="B25" s="23" t="s">
+      <c r="A25" s="21">
+        <v>21.0</v>
+      </c>
+      <c r="B25" s="22" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="8"/>
@@ -2392,7 +2389,7 @@
       <c r="AR25" s="9"/>
       <c r="AS25" s="9"/>
       <c r="AT25" s="9"/>
-      <c r="AU25" s="10" t="s">
+      <c r="AU25" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AV25" s="9"/>
@@ -2402,10 +2399,10 @@
       <c r="AZ25" s="9"/>
     </row>
     <row r="26" ht="87.75" customHeight="1">
-      <c r="A26" s="13">
-        <v>24.0</v>
-      </c>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="17">
+        <v>22.0</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="8"/>
@@ -2450,7 +2447,7 @@
       <c r="AS26" s="9"/>
       <c r="AT26" s="9"/>
       <c r="AU26" s="9"/>
-      <c r="AV26" s="10" t="s">
+      <c r="AV26" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AW26" s="9"/>
@@ -2459,10 +2456,10 @@
       <c r="AZ26" s="9"/>
     </row>
     <row r="27" ht="85.5" customHeight="1">
-      <c r="A27" s="16">
-        <v>25.0</v>
-      </c>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="18">
+        <v>23.0</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="8"/>
@@ -2513,16 +2510,16 @@
       <c r="AV27" s="9"/>
       <c r="AW27" s="9"/>
       <c r="AX27" s="9"/>
-      <c r="AY27" s="10" t="s">
+      <c r="AY27" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AZ27" s="9"/>
     </row>
     <row r="28" ht="59.25" customHeight="1">
-      <c r="A28" s="13">
-        <v>26.0</v>
-      </c>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="17">
+        <v>24.0</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="8"/>
@@ -2550,7 +2547,7 @@
       <c r="Y28" s="9"/>
       <c r="Z28" s="9"/>
       <c r="AB28" s="9"/>
-      <c r="AC28" s="10"/>
+      <c r="AC28" s="9"/>
       <c r="AD28" s="9"/>
       <c r="AE28" s="9"/>
       <c r="AF28" s="9"/>
@@ -2573,15 +2570,15 @@
       <c r="AW28" s="9"/>
       <c r="AX28" s="9"/>
       <c r="AY28" s="9"/>
-      <c r="AZ28" s="10" t="s">
+      <c r="AZ28" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" ht="61.5" customHeight="1">
-      <c r="A29" s="6">
-        <v>27.0</v>
-      </c>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="21">
+        <v>25.0</v>
+      </c>
+      <c r="B29" s="23" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="8"/>
@@ -2610,7 +2607,7 @@
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
       <c r="AB29" s="9"/>
-      <c r="AC29" s="10" t="s">
+      <c r="AC29" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AD29" s="9"/>
@@ -2627,7 +2624,7 @@
       <c r="AO29" s="9"/>
       <c r="AP29" s="9"/>
       <c r="AQ29" s="9"/>
-      <c r="AR29" s="12"/>
+      <c r="AR29" s="10"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
       <c r="AU29" s="9"/>
@@ -2638,10 +2635,10 @@
       <c r="AZ29" s="9"/>
     </row>
     <row r="30" ht="63.75" customHeight="1">
-      <c r="A30" s="13">
-        <v>28.0</v>
-      </c>
-      <c r="B30" s="25" t="s">
+      <c r="A30" s="17">
+        <v>26.0</v>
+      </c>
+      <c r="B30" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C30" s="8"/>
@@ -2670,7 +2667,7 @@
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
       <c r="AB30" s="9"/>
-      <c r="AC30" s="10" t="s">
+      <c r="AC30" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AD30" s="9"/>
@@ -2688,7 +2685,7 @@
       <c r="AP30" s="9"/>
       <c r="AQ30" s="9"/>
       <c r="AR30" s="9"/>
-      <c r="AS30" s="12"/>
+      <c r="AS30" s="10"/>
       <c r="AT30" s="9"/>
       <c r="AU30" s="9"/>
       <c r="AV30" s="9"/>
@@ -2698,10 +2695,10 @@
       <c r="AZ30" s="9"/>
     </row>
     <row r="31" ht="59.25" customHeight="1">
-      <c r="A31" s="6">
-        <v>29.0</v>
-      </c>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="21">
+        <v>27.0</v>
+      </c>
+      <c r="B31" s="23" t="s">
         <v>80</v>
       </c>
       <c r="C31" s="8"/>
@@ -2730,7 +2727,7 @@
       <c r="Z31" s="9"/>
       <c r="AA31" s="9"/>
       <c r="AB31" s="9"/>
-      <c r="AC31" s="10" t="s">
+      <c r="AC31" s="9" t="s">
         <v>68</v>
       </c>
       <c r="AD31" s="9"/>
@@ -3715,16 +3712,16 @@
     <row r="987" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Z24:Z26"/>
     <mergeCell ref="AB24:AB26"/>
     <mergeCell ref="AA27:AA28"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="L16:L17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="Y24:Y26"/>
-    <mergeCell ref="Z24:Z26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="I13:I14"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7875" footer="0.0" header="0.0" left="0.511805555555555" right="0.511805555555555" top="0.7875"/>

</xml_diff>